<commit_message>
* remove a table in the file to eliminate an exporting problem * rename a sheet to be more clear
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/conditionalFormatting.xlsx
+++ b/src/main/webapp/WEB-INF/books/conditionalFormatting.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8228C1-D044-9449-A572-BDF1166876F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F1B307-6A26-4543-9155-B192B6095DF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34680" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="903" firstSheet="3" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34680" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="903" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="36" r:id="rId1"/>
@@ -24,10 +24,10 @@
     <sheet name="Compare to totals" sheetId="33" r:id="rId14"/>
     <sheet name="Products3" sheetId="34" r:id="rId15"/>
     <sheet name="Customers2" sheetId="29" r:id="rId16"/>
-    <sheet name="Another Sheet " sheetId="37" r:id="rId17"/>
+    <sheet name="Ref to totals" sheetId="37" r:id="rId17"/>
     <sheet name="Total" sheetId="38" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="181029" calcMode="manual"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -1185,7 +1185,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1243,8 +1243,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1362,6 +1368,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1382,7 +1456,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1573,6 +1647,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="8" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1588,8 +1665,31 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="8" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1608,362 +1708,7 @@
     <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="Percent" xfId="9" builtinId="5"/>
   </cellStyles>
-  <dxfs count="76">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="double"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="&quot;$&quot;00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="175" formatCode="\(&quot;$&quot;00\)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="double"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="&quot;$&quot;00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="175" formatCode="\(&quot;$&quot;00\)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="double"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="&quot;$&quot;00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="175" formatCode="\(&quot;$&quot;00\)"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="double"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="&quot;$&quot;00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="175" formatCode="\(&quot;$&quot;00\)"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-      <numFmt numFmtId="176" formatCode="&quot;Super!  &quot;00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="\$#,##0;[Red]\$#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="\$#,##0;[Red]\$#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="double"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="&quot;$&quot;00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="175" formatCode="\(&quot;$&quot;00\)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="double"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="&quot;$&quot;00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <numFmt numFmtId="175" formatCode="\(&quot;$&quot;00\)"/>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <font>
         <b/>
@@ -2129,6 +1874,111 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="double"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <numFmt numFmtId="174" formatCode="&quot;$&quot;00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="175" formatCode="\(&quot;$&quot;00\)"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
@@ -2154,45 +2004,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2308,6 +2119,13 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2596,6 +2414,14 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <numFmt numFmtId="176" formatCode="&quot;Super!  &quot;00"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2689,6 +2515,146 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="\$#,##0;[Red]\$#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="\$#,##0;[Red]\$#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6484,32 +6450,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:E25" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:E25" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A3:E25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A3:E24">
     <sortCondition ref="A2:A24"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="City" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Date" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fee" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Attendance" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Books Sold" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="City" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Date" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fee" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Attendance" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Books Sold" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:F11" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66" dataCellStyle="Normal_Grades">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:F11" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39" dataCellStyle="Normal_Grades">
   <autoFilter ref="A2:F11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Student" dataDxfId="65" dataCellStyle="Normal_Grades"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quiz1" dataDxfId="64" dataCellStyle="Normal_Grades"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Exam1" dataDxfId="63" dataCellStyle="Normal_Grades"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Quiz2" dataDxfId="62" dataCellStyle="Normal_Grades"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Exam2" dataDxfId="61" dataCellStyle="Normal_Grades"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Grade" dataDxfId="60" dataCellStyle="Normal_Grades">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Student" dataDxfId="38" dataCellStyle="Normal_Grades"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quiz1" dataDxfId="37" dataCellStyle="Normal_Grades"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Exam1" dataDxfId="36" dataCellStyle="Normal_Grades"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Quiz2" dataDxfId="35" dataCellStyle="Normal_Grades"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Exam2" dataDxfId="34" dataCellStyle="Normal_Grades"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Grade" dataDxfId="33" dataCellStyle="Normal_Grades">
       <calculatedColumnFormula>(B3+(C3*3)+D3+(E3*3))/8</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6518,47 +6484,30 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A2:F21" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A2:F21" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A2:F21" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A2:G22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Contact Name" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Address" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="City" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Postal Code" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Country" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Phone" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Contact Name" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Address" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="City" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Postal Code" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Country" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Phone" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A3:G9" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Product"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Shifting" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Brakes" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Handle_x000a_Bars" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Seat" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Frequency_x000a_of Repair" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Overall_x000a_Score" dataDxfId="44">
-      <calculatedColumnFormula>AVERAGE(B4:F4)</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table4" displayName="Table4" ref="A2:C14" totalsRowShown="0">
   <autoFilter ref="A2:C14" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="FY 2008"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Profits" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Trend" dataDxfId="42">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Profits" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Trend" dataDxfId="22">
       <calculatedColumnFormula>B3-B2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6566,31 +6515,31 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A3:B12" totalsRowCount="1">
   <autoFilter ref="A3:B11" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Region" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Sales" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Sales" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table38" displayName="Table38" ref="A2:H20" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table38" displayName="Table38" ref="A2:H20" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A2:H20" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Contact Name" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Address" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="City" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Postal Code" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Country" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Phone" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="#" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Contact Name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Address" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="City" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Postal Code" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Country" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Phone" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="#" dataDxfId="3">
       <calculatedColumnFormula>COUNTIFS($A$3:$A$20,A3,$B$3:$B$20,B3,$C$3:$C$20,C3,$D$3:$D$20,D3,$E$3:$E$20,E3, $F$3:$F$20,F3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="T/F" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="T/F" dataDxfId="2">
       <calculatedColumnFormula>NOT(IF(G3&gt;1,TRUE,FALSE))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6945,16 +6894,16 @@
       <c r="B4" s="47"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="97" t="s">
         <v>298</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
     </row>
     <row r="6" spans="1:4" ht="17.25" customHeight="1">
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
+      <c r="B6" s="97"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" s="75"/>
@@ -6973,7 +6922,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="96" t="s">
         <v>302</v>
       </c>
       <c r="C9" s="72" t="s">
@@ -6984,7 +6933,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="96" t="s">
         <v>303</v>
       </c>
       <c r="C10" s="72" t="s">
@@ -6995,7 +6944,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="32">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="96" t="s">
         <v>304</v>
       </c>
       <c r="C11" s="73" t="s">
@@ -7006,7 +6955,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="96" t="s">
         <v>305</v>
       </c>
       <c r="C12" s="73" t="s">
@@ -7017,7 +6966,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="96" t="s">
         <v>306</v>
       </c>
       <c r="C13" s="73" t="s">
@@ -7028,7 +6977,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="96" t="s">
         <v>307</v>
       </c>
       <c r="C14" s="74" t="s">
@@ -7039,7 +6988,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="96" t="s">
         <v>308</v>
       </c>
       <c r="C15" s="74" t="s">
@@ -7050,7 +6999,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="B16" s="101" t="s">
+      <c r="B16" s="96" t="s">
         <v>309</v>
       </c>
       <c r="C16" s="74" t="s">
@@ -7061,7 +7010,7 @@
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="96" t="s">
         <v>310</v>
       </c>
       <c r="C17" s="74" t="s">
@@ -7072,7 +7021,7 @@
       </c>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="96" t="s">
         <v>311</v>
       </c>
       <c r="C18" s="74" t="s">
@@ -7083,7 +7032,7 @@
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="101" t="s">
+      <c r="B19" s="96" t="s">
         <v>312</v>
       </c>
       <c r="C19" s="72" t="s">
@@ -7094,7 +7043,7 @@
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="101" t="s">
+      <c r="B20" s="96" t="s">
         <v>313</v>
       </c>
       <c r="C20" s="74" t="s">
@@ -7105,7 +7054,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="16">
-      <c r="B21" s="101" t="s">
+      <c r="B21" s="96" t="s">
         <v>314</v>
       </c>
       <c r="C21" s="74" t="s">
@@ -7116,7 +7065,7 @@
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="96" t="s">
         <v>315</v>
       </c>
       <c r="C22" s="74" t="s">
@@ -7127,7 +7076,7 @@
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="101" t="s">
+      <c r="B23" s="96" t="s">
         <v>316</v>
       </c>
       <c r="C23" s="74" t="s">
@@ -7306,7 +7255,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13"/>
@@ -7345,10 +7294,10 @@
       <c r="G2" s="85" t="s">
         <v>282</v>
       </c>
-      <c r="H2" s="98" t="s">
+      <c r="H2" s="99" t="s">
         <v>294</v>
       </c>
-      <c r="I2" s="99"/>
+      <c r="I2" s="100"/>
       <c r="J2" s="86"/>
       <c r="K2" s="86"/>
     </row>
@@ -9013,21 +8962,21 @@
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10">
       <c r="A2" s="60"/>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="101" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100" t="s">
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101" t="s">
         <v>224</v>
       </c>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100" t="s">
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101" t="s">
         <v>225</v>
       </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="60" t="s">
@@ -9838,7 +9787,7 @@
     <mergeCell ref="H2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:J25">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10476,10 +10425,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:E17">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>B4&lt;=$F4*0.2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>B4&gt;=$F4*0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11155,22 +11104,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A23">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>AND(MONTH(A3)=MONTH(TODAY()),B3="Grain",D3&lt;500)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B23">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>AND(B3="Grain",MONTH(A3)=MONTH(TODAY()),D3&lt;500)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D24">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>AND(D3&lt;500,B3="Grain",MONTH(A3)=MONTH(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C23">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>AND(C3=C3,B3="Grain",MONTH(A3)=MONTH(TODAY()),D3&lt;500)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11791,7 +11740,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:H20">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>AND(A3:H3)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11808,7 +11757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8870E63-F583-C14E-9D94-76DD070C1310}">
   <dimension ref="A2:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
@@ -12431,7 +12380,7 @@
         <v>95</v>
       </c>
       <c r="B4" s="46">
-        <f>SUM('Another Sheet '!B4:E4)</f>
+        <f>SUM('Ref to totals'!B4:E4)</f>
         <v>220</v>
       </c>
     </row>
@@ -12440,7 +12389,7 @@
         <v>189</v>
       </c>
       <c r="B5" s="46">
-        <f>SUM('Another Sheet '!B5:E5)</f>
+        <f>SUM('Ref to totals'!B5:E5)</f>
         <v>323</v>
       </c>
     </row>
@@ -12449,7 +12398,7 @@
         <v>97</v>
       </c>
       <c r="B6" s="46">
-        <f>SUM('Another Sheet '!B6:E6)</f>
+        <f>SUM('Ref to totals'!B6:E6)</f>
         <v>270</v>
       </c>
     </row>
@@ -12458,7 +12407,7 @@
         <v>185</v>
       </c>
       <c r="B7" s="46">
-        <f>SUM('Another Sheet '!B7:E7)</f>
+        <f>SUM('Ref to totals'!B7:E7)</f>
         <v>282</v>
       </c>
     </row>
@@ -12473,7 +12422,7 @@
         <v>95</v>
       </c>
       <c r="B9" s="46">
-        <f>SUM('Another Sheet '!B9:E9)</f>
+        <f>SUM('Ref to totals'!B9:E9)</f>
         <v>243</v>
       </c>
     </row>
@@ -12482,7 +12431,7 @@
         <v>189</v>
       </c>
       <c r="B10" s="46">
-        <f>SUM('Another Sheet '!B10:E10)</f>
+        <f>SUM('Ref to totals'!B10:E10)</f>
         <v>281</v>
       </c>
     </row>
@@ -12491,7 +12440,7 @@
         <v>97</v>
       </c>
       <c r="B11" s="46">
-        <f>SUM('Another Sheet '!B11:E11)</f>
+        <f>SUM('Ref to totals'!B11:E11)</f>
         <v>284</v>
       </c>
     </row>
@@ -12500,7 +12449,7 @@
         <v>185</v>
       </c>
       <c r="B12" s="46">
-        <f>SUM('Another Sheet '!B12:E12)</f>
+        <f>SUM('Ref to totals'!B12:E12)</f>
         <v>282</v>
       </c>
     </row>
@@ -12515,7 +12464,7 @@
         <v>95</v>
       </c>
       <c r="B14" s="46">
-        <f>SUM('Another Sheet '!B14:E14)</f>
+        <f>SUM('Ref to totals'!B14:E14)</f>
         <v>291</v>
       </c>
     </row>
@@ -12524,7 +12473,7 @@
         <v>189</v>
       </c>
       <c r="B15" s="46">
-        <f>SUM('Another Sheet '!B15:E15)</f>
+        <f>SUM('Ref to totals'!B15:E15)</f>
         <v>249</v>
       </c>
     </row>
@@ -12533,7 +12482,7 @@
         <v>97</v>
       </c>
       <c r="B16" s="46">
-        <f>SUM('Another Sheet '!B16:E16)</f>
+        <f>SUM('Ref to totals'!B16:E16)</f>
         <v>312</v>
       </c>
     </row>
@@ -12542,7 +12491,7 @@
         <v>185</v>
       </c>
       <c r="B17" s="46">
-        <f>SUM('Another Sheet '!B17:E17)</f>
+        <f>SUM('Ref to totals'!B17:E17)</f>
         <v>289</v>
       </c>
     </row>
@@ -13192,17 +13141,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A23">
-    <cfRule type="timePeriod" dxfId="23" priority="3" timePeriod="thisMonth">
+    <cfRule type="timePeriod" dxfId="57" priority="3" timePeriod="thisMonth">
       <formula>AND(MONTH(A3)=MONTH(TODAY()),YEAR(A3)=YEAR(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B23">
-    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="Grain">
+    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Grain">
       <formula>NOT(ISERROR(SEARCH("Grain",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D23">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="lessThan">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13222,7 +13171,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -13879,12 +13830,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B24">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D24">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="9" operator="lessThan">
       <formula>$G$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14656,13 +14607,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C25">
-    <cfRule type="top10" dxfId="18" priority="6" percent="1" rank="20"/>
+    <cfRule type="top10" dxfId="52" priority="6" percent="1" rank="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E25">
-    <cfRule type="top10" dxfId="17" priority="5" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="51" priority="5" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D25">
-    <cfRule type="aboveAverage" dxfId="16" priority="4"/>
+    <cfRule type="aboveAverage" dxfId="50" priority="4"/>
   </conditionalFormatting>
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14684,7 +14635,7 @@
   <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14908,7 +14859,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F11">
-    <cfRule type="top10" dxfId="15" priority="1" rank="2"/>
+    <cfRule type="top10" dxfId="42" priority="1" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -15392,7 +15343,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A21">
-    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15703,20 +15654,20 @@
       <c r="B2" s="58">
         <v>2005</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="98" t="s">
         <v>288</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
       <c r="O2" s="26"/>
       <c r="P2" s="26"/>
       <c r="Q2" s="26"/>
@@ -16164,8 +16115,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -16196,168 +16147,168 @@
       <c r="G2" s="53"/>
     </row>
     <row r="3" spans="1:7" ht="32">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="103" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="103" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="104" t="s">
         <v>255</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="103" t="s">
         <v>175</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="104" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="105" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="A4" s="106" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="107">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="107">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="107">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="107">
         <v>2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="107">
         <v>3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="108">
         <f>AVERAGE(B4:F4)</f>
         <v>2.4</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="A5" s="106" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="107">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="107">
         <v>3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="107">
         <v>3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="107">
         <v>5</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="107">
         <v>4</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="108">
         <f t="shared" ref="G5:G9" si="0">AVERAGE(B5:F5)</f>
         <v>3.8</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="A6" s="106" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="107">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="107">
         <v>3</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="107">
         <v>3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="107">
         <v>3</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="107">
         <v>2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="108">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="A7" s="106" t="s">
         <v>177</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="107">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="107">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="107">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="107">
         <v>2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="107">
         <v>1</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="108">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="A8" s="106" t="s">
         <v>178</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="107">
         <v>2</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="107">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="107">
         <v>3</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="107">
         <v>4</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="107">
         <v>2</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="108">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="A9" s="109" t="s">
         <v>179</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="110">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="110">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="110">
         <v>2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="110">
         <v>1</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="110">
         <v>5</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="111">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
@@ -16396,9 +16347,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>